<commit_message>
Added code for LTPC_Adder.py
</commit_message>
<xml_diff>
--- a/Timetable/new_mal_4.xlsx
+++ b/Timetable/new_mal_4.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>[0. 0. 2. 2.]</t>
+          <t>[0. 0. 3. 2.]</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>[2. 2. 0. 0.]</t>
+          <t>[3. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -2956,7 +2956,7 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -3381,7 +3381,7 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -5110,7 +5110,7 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>[2. 0. 2. 0.]</t>
+          <t>[3. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>[2. 2. 0. 0.]</t>
+          <t>[3. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="R116" t="inlineStr">
         <is>
-          <t>[2. 0. 0. 0.]</t>
+          <t>[3. 0. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="R121" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -7279,7 +7279,7 @@
       </c>
       <c r="R124" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -7401,7 +7401,7 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 1. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -9886,7 +9886,7 @@
       </c>
       <c r="R165" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 2. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -10157,7 +10157,7 @@
       </c>
       <c r="R170" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 2. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -10656,7 +10656,7 @@
       </c>
       <c r="R179" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 2. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -14219,7 +14219,7 @@
       </c>
       <c r="R236" t="inlineStr">
         <is>
-          <t>[0. 0. 2. 0.]</t>
+          <t>[0. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -15826,7 +15826,7 @@
       </c>
       <c r="R261" t="inlineStr">
         <is>
-          <t>[0. 0. 2. 0.]</t>
+          <t>[0. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -16926,7 +16926,7 @@
       </c>
       <c r="R283" t="inlineStr">
         <is>
-          <t>[2. 2. 0. 0.]</t>
+          <t>[3. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -17659,7 +17659,7 @@
       </c>
       <c r="R298" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -17781,7 +17781,7 @@
       </c>
       <c r="R300" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -17903,7 +17903,7 @@
       </c>
       <c r="R302" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -18025,7 +18025,7 @@
       </c>
       <c r="R304" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -18206,7 +18206,7 @@
       </c>
       <c r="R307" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -18328,7 +18328,7 @@
       </c>
       <c r="R309" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -18450,7 +18450,7 @@
       </c>
       <c r="R311" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 1. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -19543,7 +19543,7 @@
       </c>
       <c r="R328" t="inlineStr">
         <is>
-          <t>[2. 0. 2. 2.]</t>
+          <t>[3. 0. 3. 2.]</t>
         </is>
       </c>
     </row>
@@ -20259,7 +20259,7 @@
       </c>
       <c r="R342" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -20891,7 +20891,7 @@
       </c>
       <c r="R354" t="inlineStr">
         <is>
-          <t>[2. 2. 2. 0.]</t>
+          <t>[2. 3. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -22032,7 +22032,7 @@
       </c>
       <c r="R375" t="inlineStr">
         <is>
-          <t>[2. 0. 2. 0.]</t>
+          <t>[2. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -23281,7 +23281,7 @@
       </c>
       <c r="R398" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -24534,7 +24534,7 @@
       </c>
       <c r="R417" t="inlineStr">
         <is>
-          <t>[2. 2. 0. 0.]</t>
+          <t>[3. 2. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -25147,7 +25147,7 @@
       </c>
       <c r="R428" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -26210,7 +26210,7 @@
       </c>
       <c r="R445" t="inlineStr">
         <is>
-          <t>[2. 2. 0. 0.]</t>
+          <t>[3. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -26990,7 +26990,7 @@
       </c>
       <c r="R461" t="inlineStr">
         <is>
-          <t>[2. 2. 2. 0.]</t>
+          <t>[2. 3. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -28263,7 +28263,7 @@
       </c>
       <c r="R486" t="inlineStr">
         <is>
-          <t>[2. 2. 2. 0.]</t>
+          <t>[2. 3. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -29187,7 +29187,7 @@
       </c>
       <c r="R504" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 3. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -30710,7 +30710,7 @@
       </c>
       <c r="R531" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -32685,7 +32685,7 @@
       </c>
       <c r="R560" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -34157,7 +34157,7 @@
       </c>
       <c r="R582" t="inlineStr">
         <is>
-          <t>[2. 2. 2. 0.]</t>
+          <t>[2. 3. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -35430,7 +35430,7 @@
       </c>
       <c r="R607" t="inlineStr">
         <is>
-          <t>[2. 2. 2. 0.]</t>
+          <t>[2. 3. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -36285,7 +36285,7 @@
       </c>
       <c r="R624" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -37470,7 +37470,7 @@
       </c>
       <c r="R645" t="inlineStr">
         <is>
-          <t>[2. 2. 0. 0.]</t>
+          <t>[3. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -38775,7 +38775,7 @@
       </c>
       <c r="R672" t="inlineStr">
         <is>
-          <t>[2. 0. 0. 2.]</t>
+          <t>[3. 0. 0. 2.]</t>
         </is>
       </c>
     </row>
@@ -39506,7 +39506,7 @@
       </c>
       <c r="R685" t="inlineStr">
         <is>
-          <t>[2. 2. 0. 0.]</t>
+          <t>[2. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -39816,7 +39816,7 @@
       </c>
       <c r="R691" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -39985,7 +39985,7 @@
       </c>
       <c r="R694" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -40107,7 +40107,7 @@
       </c>
       <c r="R696" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -40288,7 +40288,7 @@
       </c>
       <c r="R699" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -40457,7 +40457,7 @@
       </c>
       <c r="R702" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -40626,7 +40626,7 @@
       </c>
       <c r="R705" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -43024,7 +43024,7 @@
       </c>
       <c r="R741" t="inlineStr">
         <is>
-          <t>[0. 0. 2. 0.]</t>
+          <t>[0. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -44580,7 +44580,7 @@
       </c>
       <c r="R771" t="inlineStr">
         <is>
-          <t>[0. 0. 2. 0.]</t>
+          <t>[0. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -44906,7 +44906,7 @@
       </c>
       <c r="R777" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -45442,7 +45442,7 @@
       </c>
       <c r="R787" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -46909,7 +46909,7 @@
       </c>
       <c r="R810" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -48681,7 +48681,7 @@
       </c>
       <c r="R842" t="inlineStr">
         <is>
-          <t>[0. 0. 2. 0.]</t>
+          <t>[0. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -49007,7 +49007,7 @@
       </c>
       <c r="R848" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -49304,7 +49304,7 @@
       </c>
       <c r="R853" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -50127,7 +50127,7 @@
       </c>
       <c r="R866" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 1. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -50351,7 +50351,7 @@
       </c>
       <c r="R870" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 1. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -50634,7 +50634,7 @@
       </c>
       <c r="R875" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 1. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -50858,7 +50858,7 @@
       </c>
       <c r="R879" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 1. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -51082,7 +51082,7 @@
       </c>
       <c r="R883" t="inlineStr">
         <is>
-          <t>[2. 2. 2. 0.]</t>
+          <t>[3. 3. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -51400,7 +51400,7 @@
       </c>
       <c r="R889" t="inlineStr">
         <is>
-          <t>[1. 2. 2. 0.]</t>
+          <t>[1. 1. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -52055,7 +52055,7 @@
       </c>
       <c r="R900" t="inlineStr">
         <is>
-          <t>[1. 0. 2. 0.]</t>
+          <t>[1. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -53851,7 +53851,7 @@
       </c>
       <c r="R928" t="inlineStr">
         <is>
-          <t>[0. 0. 2. 0.]</t>
+          <t>[0. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -54951,7 +54951,7 @@
       </c>
       <c r="R950" t="inlineStr">
         <is>
-          <t>[2. 2. 0. 0.]</t>
+          <t>[3. 3. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -55684,7 +55684,7 @@
       </c>
       <c r="R965" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -55806,7 +55806,7 @@
       </c>
       <c r="R967" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -56144,7 +56144,7 @@
       </c>
       <c r="R973" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -56264,7 +56264,7 @@
       </c>
       <c r="R975" t="inlineStr">
         <is>
-          <t>[0. 0. 2. 0.]</t>
+          <t>[0. 0. 3. 0.]</t>
         </is>
       </c>
     </row>
@@ -56443,7 +56443,7 @@
       </c>
       <c r="R978" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -56565,7 +56565,7 @@
       </c>
       <c r="R980" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>
@@ -56687,7 +56687,7 @@
       </c>
       <c r="R982" t="inlineStr">
         <is>
-          <t>[1. 2. 0. 0.]</t>
+          <t>[1. 1. 0. 0.]</t>
         </is>
       </c>
     </row>

</xml_diff>